<commit_message>
Forgot to save spreadsheet.
</commit_message>
<xml_diff>
--- a/notebook/20190626_purify_zif268_repa_via_ribosome_pull_down/nanodrop.xlsx
+++ b/notebook/20190626_purify_zif268_repa_via_ribosome_pull_down/nanodrop.xlsx
@@ -91,7 +91,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -165,6 +165,9 @@
       </c>
       <c r="B5" t="s">
         <v>0</v>
+      </c>
+      <c r="C5">
+        <v>286.80000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>